<commit_message>
update sweep dyn master
</commit_message>
<xml_diff>
--- a/isobxr/inst/extdata/0_SWEEP_DYN_MASTER.xlsx
+++ b/isobxr/inst/extdata/0_SWEEP_DYN_MASTER.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sz18642/OneDrive - University of Bristol/5_isobxr/tutorials/7_sweep_perturbation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sz18642/isobxr/isobxr/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F7A1E15-6582-1748-A16C-E46A1DDC8F9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99D86FA-BCD5-5344-AD96-A604907B2EB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="440" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{A8BCD4FD-523E-B84B-BCD1-532558DEDCF9}"/>
+    <workbookView xWindow="2520" yWindow="460" windowWidth="28800" windowHeight="18000" xr2:uid="{A8BCD4FD-523E-B84B-BCD1-532558DEDCF9}"/>
   </bookViews>
   <sheets>
     <sheet name="RUN_LIST" sheetId="1" r:id="rId1"/>
@@ -471,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A616C602-63C1-6449-9F9C-65D79D28DEBF}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -523,7 +523,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4">
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="C3" s="4">
         <v>1000</v>
@@ -696,7 +696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C50A76E4-F6AD-A64A-BE18-B4A929BAE54B}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>